<commit_message>
Added font handling to chart data labels.
</commit_message>
<xml_diff>
--- a/xlsxwriter/test/comparison/xlsx_files/chart_data_labels21.xlsx
+++ b/xlsxwriter/test/comparison/xlsx_files/chart_data_labels21.xlsx
@@ -68,6 +68,18 @@
           <c:order val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
             <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="1"/>
             <c:showVal val="1"/>
@@ -123,7 +135,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>

</xml_diff>